<commit_message>
Processed Results - nexus 5x until https request
</commit_message>
<xml_diff>
--- a/Processed Results/Nexus 5X/Gravity/Gravity - Processed.xlsx
+++ b/Processed Results/Nexus 5X/Gravity/Gravity - Processed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Nexus 5X\Gravity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0253038-2A08-4369-B950-5A8A0E16568B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8181C1BA-4B3F-4BEA-9F7E-3FD7AD5A6E2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
+    <workbookView xWindow="130" yWindow="120" windowWidth="9990" windowHeight="9830" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Blad1!$A$2:$A$31</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$2:$B$31</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$2:$A$31</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$2:$B$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -257,94 +259,94 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>101.631671999999</c:v>
+                  <c:v>116.067275999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.904056</c:v>
+                  <c:v>119.82653999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.745008</c:v>
+                  <c:v>119.983176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>102.745008</c:v>
+                  <c:v>119.82653999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>101.154528</c:v>
+                  <c:v>119.82653999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>102.108816</c:v>
+                  <c:v>121.079628</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>102.904056</c:v>
+                  <c:v>119.043359999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>103.54024800000001</c:v>
+                  <c:v>119.82653999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>102.904056</c:v>
+                  <c:v>120.296448</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>102.26786399999899</c:v>
+                  <c:v>121.236263999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>102.745008</c:v>
+                  <c:v>119.983176</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>102.26786399999899</c:v>
+                  <c:v>116.067275999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>102.426912</c:v>
+                  <c:v>121.3929</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>104.81263199999999</c:v>
+                  <c:v>118.260179999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>102.26786399999899</c:v>
+                  <c:v>120.453084</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>99.723095999999899</c:v>
+                  <c:v>119.199996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>102.108816</c:v>
+                  <c:v>119.82653999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>102.426912</c:v>
+                  <c:v>119.199996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>102.58596</c:v>
+                  <c:v>119.356632</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>101.94976800000001</c:v>
+                  <c:v>120.766356</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>102.58596</c:v>
+                  <c:v>120.296448</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>102.426912</c:v>
+                  <c:v>119.669904</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>102.108816</c:v>
+                  <c:v>121.236263999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>102.26786399999899</c:v>
+                  <c:v>119.043359999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>102.426912</c:v>
+                  <c:v>120.60972</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>102.108816</c:v>
+                  <c:v>120.453084</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>103.063104</c:v>
+                  <c:v>121.549536</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>102.26786399999899</c:v>
+                  <c:v>119.356632</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>102.904056</c:v>
+                  <c:v>114.814188</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>102.26786399999899</c:v>
+                  <c:v>122.01944399999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,10 +422,10 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>102.42161039999972</c:v>
+                  <c:v>119.68556759999979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.42161039999972</c:v>
+                  <c:v>119.68556759999979</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -574,7 +576,6 @@
         <c:axId val="509815096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="105"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -827,7 +828,7 @@
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
-        <cx:valScaling max="105" min="99"/>
+        <cx:valScaling max="123" min="114"/>
         <cx:title>
           <cx:tx>
             <cx:txData>
@@ -2395,12 +2396,13 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B6" activeCellId="4" sqref="B2 B3 B5 B4 B6:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.90625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2417,7 +2419,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>101.631671999999</v>
+        <v>116.067275999999</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
@@ -2431,14 +2433,14 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>102.904056</v>
+        <v>119.82653999999999</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>102.42161039999972</v>
+        <v>119.68556759999979</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2446,14 +2448,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>102.745008</v>
+        <v>119.983176</v>
       </c>
       <c r="D4">
         <v>30</v>
       </c>
       <c r="E4" s="1">
         <f>AVERAGE(B2,B3,B4,B5,B6,B7,B8,B9,B10,B11,B12,B13,B14,B15,B16,B17,B18,B19,B21,B20,B22,B23,B24,B25,B26,B27,B28,B29,B30,B31)</f>
-        <v>102.42161039999972</v>
+        <v>119.68556759999979</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -2461,7 +2463,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>102.745008</v>
+        <v>119.82653999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2469,7 +2471,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>101.154528</v>
+        <v>119.82653999999999</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>4</v>
@@ -2483,15 +2485,15 @@
         <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>102.108816</v>
+        <v>121.079628</v>
       </c>
       <c r="D7" s="1">
         <f>MIN(B2:B31)</f>
-        <v>99.723095999999899</v>
+        <v>114.814188</v>
       </c>
       <c r="E7" s="1">
         <f>MAX(B2:B31)</f>
-        <v>104.81263199999999</v>
+        <v>122.01944399999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2499,7 +2501,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>102.904056</v>
+        <v>119.043359999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2507,7 +2509,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>103.54024800000001</v>
+        <v>119.82653999999999</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
@@ -2521,15 +2523,15 @@
         <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>102.904056</v>
+        <v>120.296448</v>
       </c>
       <c r="D10">
         <f>QUARTILE(B2:B31, 1)</f>
-        <v>102.14857799999976</v>
+        <v>119.239155</v>
       </c>
       <c r="E10">
         <f>QUARTILE(B2:B31, 2)</f>
-        <v>102.426912</v>
+        <v>119.82653999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2537,7 +2539,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1">
-        <v>102.26786399999899</v>
+        <v>121.236263999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2545,7 +2547,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>102.745008</v>
+        <v>119.983176</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -2559,15 +2561,15 @@
         <v>3</v>
       </c>
       <c r="B13" s="1">
-        <v>102.26786399999899</v>
+        <v>116.067275999999</v>
       </c>
       <c r="D13">
         <f>QUARTILE(B2:B31, 3)</f>
-        <v>102.745008</v>
+        <v>120.570561</v>
       </c>
       <c r="E13">
         <f xml:space="preserve"> D13 - D10</f>
-        <v>0.5964300000002396</v>
+        <v>1.3314060000000012</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2575,7 +2577,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="1">
-        <v>102.426912</v>
+        <v>121.3929</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -2583,7 +2585,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1">
-        <v>104.81263199999999</v>
+        <v>118.260179999999</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>10</v>
@@ -2597,15 +2599,15 @@
         <v>3</v>
       </c>
       <c r="B16" s="1">
-        <v>102.26786399999899</v>
+        <v>120.453084</v>
       </c>
       <c r="D16">
         <f>STDEV(B2:B31)</f>
-        <v>0.80827744154537839</v>
+        <v>1.6217428493713799</v>
       </c>
       <c r="E16">
         <f xml:space="preserve"> (D16 / E4) * 100</f>
-        <v>0.78916689396770179</v>
+        <v>1.3550028477881262</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -2613,7 +2615,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="1">
-        <v>99.723095999999899</v>
+        <v>119.199996</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -2621,7 +2623,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="1">
-        <v>102.108816</v>
+        <v>119.82653999999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -2629,7 +2631,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="1">
-        <v>102.426912</v>
+        <v>119.199996</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -2637,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="1">
-        <v>102.58596</v>
+        <v>119.356632</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -2645,7 +2647,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="1">
-        <v>101.94976800000001</v>
+        <v>120.766356</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -2653,7 +2655,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="1">
-        <v>102.58596</v>
+        <v>120.296448</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -2661,7 +2663,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="1">
-        <v>102.426912</v>
+        <v>119.669904</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -2669,7 +2671,7 @@
         <v>3</v>
       </c>
       <c r="B24" s="1">
-        <v>102.108816</v>
+        <v>121.236263999999</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -2677,7 +2679,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="1">
-        <v>102.26786399999899</v>
+        <v>119.043359999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -2685,7 +2687,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="1">
-        <v>102.426912</v>
+        <v>120.60972</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -2693,7 +2695,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="1">
-        <v>102.108816</v>
+        <v>120.453084</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -2701,7 +2703,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="1">
-        <v>103.063104</v>
+        <v>121.549536</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -2709,7 +2711,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="1">
-        <v>102.26786399999899</v>
+        <v>119.356632</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -2717,7 +2719,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="1">
-        <v>102.904056</v>
+        <v>114.814188</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -2725,7 +2727,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="1">
-        <v>102.26786399999899</v>
+        <v>122.01944399999999</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>